<commit_message>
Remove Github merge lines
</commit_message>
<xml_diff>
--- a/vignettes/retail.xlsx
+++ b/vignettes/retail.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johannes Schnebel\Documents\IFW\ifwtrends\vignettes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cb9e74139d05168d/IfW/ifwtrends/vignettes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D6375A-6738-4D59-A83A-D42F3769CAE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{25D6375A-6738-4D59-A83A-D42F3769CAE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37704BF2-2CCA-4806-9F27-307B0C71CE33}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -101,9 +101,9 @@
   <volType type="realTimeData">
     <main first="refinitivshim.rtdserver.dsgrid">
       <tp t="s">
-        <v>Name</v>
+        <v>Not Signed In</v>
         <stp/>
-        <stp>{92696FB6-2386-4542-83A5-117CE85C957B}</stp>
+        <stp>{73873DF9-62F1-4DA4-BD3D-B74A13437590}</stp>
         <tr r="A1" s="1"/>
       </tp>
     </main>
@@ -378,21 +378,21 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="str">
         <f>_xll.DSGRID("BDRETTOTG"," ","2006-01-01"," ","M","RowHeader=true;ColHeader=true;DispSeriesDescription=true;YearlyTSFormat=false;QuarterlyTSFormat=false")</f>
-        <v>Name</v>
+        <v>Not Signed In</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>38732</v>
       </c>
@@ -400,7 +400,7 @@
         <v>96.4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>38763</v>
       </c>
@@ -408,7 +408,7 @@
         <v>96.7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>38791</v>
       </c>
@@ -416,7 +416,7 @@
         <v>96.3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>38822</v>
       </c>
@@ -424,7 +424,7 @@
         <v>96.8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>38852</v>
       </c>
@@ -432,7 +432,7 @@
         <v>97.2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>38883</v>
       </c>
@@ -440,7 +440,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>38913</v>
       </c>
@@ -448,7 +448,7 @@
         <v>96.3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>38944</v>
       </c>
@@ -456,7 +456,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>38975</v>
       </c>
@@ -464,7 +464,7 @@
         <v>95.5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>39005</v>
       </c>
@@ -472,7 +472,7 @@
         <v>96.2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>39036</v>
       </c>
@@ -480,7 +480,7 @@
         <v>96.3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>39066</v>
       </c>
@@ -488,7 +488,7 @@
         <v>100.7</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>39097</v>
       </c>
@@ -496,7 +496,7 @@
         <v>94.6</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>39128</v>
       </c>
@@ -504,7 +504,7 @@
         <v>96.6</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>39156</v>
       </c>
@@ -512,7 +512,7 @@
         <v>96.5</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>39187</v>
       </c>
@@ -520,7 +520,7 @@
         <v>99.2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>39217</v>
       </c>
@@ -528,7 +528,7 @@
         <v>94.3</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>39248</v>
       </c>
@@ -536,7 +536,7 @@
         <v>95.4</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>39278</v>
       </c>
@@ -544,7 +544,7 @@
         <v>95.5</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>39309</v>
       </c>
@@ -552,7 +552,7 @@
         <v>95.5</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>39340</v>
       </c>
@@ -560,7 +560,7 @@
         <v>95.7</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>39370</v>
       </c>
@@ -568,7 +568,7 @@
         <v>95.6</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>39401</v>
       </c>
@@ -576,7 +576,7 @@
         <v>94.5</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>39431</v>
       </c>
@@ -584,7 +584,7 @@
         <v>94.7</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>39462</v>
       </c>
@@ -592,7 +592,7 @@
         <v>95.7</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>39493</v>
       </c>
@@ -600,7 +600,7 @@
         <v>96.6</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>39522</v>
       </c>
@@ -608,7 +608,7 @@
         <v>94.8</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>39553</v>
       </c>
@@ -616,7 +616,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>39583</v>
       </c>
@@ -624,7 +624,7 @@
         <v>94.8</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>39614</v>
       </c>
@@ -632,7 +632,7 @@
         <v>94.2</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>39644</v>
       </c>
@@ -640,7 +640,7 @@
         <v>94.2</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>39675</v>
       </c>
@@ -648,7 +648,7 @@
         <v>95.1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>39706</v>
       </c>
@@ -656,7 +656,7 @@
         <v>96.6</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>39736</v>
       </c>
@@ -664,7 +664,7 @@
         <v>95.3</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>39767</v>
       </c>
@@ -672,7 +672,7 @@
         <v>96.1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>39797</v>
       </c>
@@ -680,7 +680,7 @@
         <v>95.9</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>39828</v>
       </c>
@@ -688,7 +688,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>39859</v>
       </c>
@@ -696,7 +696,7 @@
         <v>92.6</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>39887</v>
       </c>
@@ -704,7 +704,7 @@
         <v>92.7</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>39918</v>
       </c>
@@ -712,7 +712,7 @@
         <v>94.7</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>39948</v>
       </c>
@@ -720,7 +720,7 @@
         <v>92.2</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>39979</v>
       </c>
@@ -728,7 +728,7 @@
         <v>90.7</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>40009</v>
       </c>
@@ -736,7 +736,7 @@
         <v>92.5</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>40040</v>
       </c>
@@ -744,7 +744,7 @@
         <v>91.6</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>40071</v>
       </c>
@@ -752,7 +752,7 @@
         <v>92.6</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>40101</v>
       </c>
@@ -760,7 +760,7 @@
         <v>92.9</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>40132</v>
       </c>
@@ -768,7 +768,7 @@
         <v>93.3</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>40162</v>
       </c>
@@ -776,7 +776,7 @@
         <v>93.9</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>40193</v>
       </c>
@@ -784,7 +784,7 @@
         <v>91.2</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>40224</v>
       </c>
@@ -792,7 +792,7 @@
         <v>93.4</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>40252</v>
       </c>
@@ -800,7 +800,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>40283</v>
       </c>
@@ -808,7 +808,7 @@
         <v>93.6</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>40313</v>
       </c>
@@ -816,7 +816,7 @@
         <v>94.1</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>40344</v>
       </c>
@@ -824,7 +824,7 @@
         <v>94.6</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>40374</v>
       </c>
@@ -832,7 +832,7 @@
         <v>95.3</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>40405</v>
       </c>
@@ -840,7 +840,7 @@
         <v>94.6</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>40436</v>
       </c>
@@ -848,7 +848,7 @@
         <v>94.2</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>40466</v>
       </c>
@@ -856,7 +856,7 @@
         <v>93.9</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>40497</v>
       </c>
@@ -864,7 +864,7 @@
         <v>94.1</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>40527</v>
       </c>
@@ -872,7 +872,7 @@
         <v>93.7</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>40558</v>
       </c>
@@ -880,7 +880,7 @@
         <v>94.3</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>40589</v>
       </c>
@@ -888,7 +888,7 @@
         <v>96.2</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>40617</v>
       </c>
@@ -896,7 +896,7 @@
         <v>93.7</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>40648</v>
       </c>
@@ -904,7 +904,7 @@
         <v>95.2</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>40678</v>
       </c>
@@ -912,7 +912,7 @@
         <v>92.6</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>40709</v>
       </c>
@@ -920,7 +920,7 @@
         <v>95.1</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>40739</v>
       </c>
@@ -928,7 +928,7 @@
         <v>95.5</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>40770</v>
       </c>
@@ -936,7 +936,7 @@
         <v>95.5</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>40801</v>
       </c>
@@ -944,7 +944,7 @@
         <v>95.1</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>40831</v>
       </c>
@@ -952,7 +952,7 @@
         <v>95.7</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>40862</v>
       </c>
@@ -960,7 +960,7 @@
         <v>94.9</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>40892</v>
       </c>
@@ -968,7 +968,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>40923</v>
       </c>
@@ -976,7 +976,7 @@
         <v>93.8</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>40954</v>
       </c>
@@ -984,7 +984,7 @@
         <v>94.4</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>40983</v>
       </c>
@@ -992,7 +992,7 @@
         <v>95.1</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>41014</v>
       </c>
@@ -1000,7 +1000,7 @@
         <v>95.2</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>41044</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>94.9</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>41075</v>
       </c>
@@ -1016,7 +1016,7 @@
         <v>95.7</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>41105</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>94.8</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>41136</v>
       </c>
@@ -1032,7 +1032,7 @@
         <v>94.8</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>41167</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>95.3</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>41197</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>41228</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>94.5</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>41258</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>94.9</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>41289</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>95.4</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>41320</v>
       </c>
@@ -1080,7 +1080,7 @@
         <v>94.8</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>41348</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>95.2</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>41379</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>94.9</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>41409</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>95.5</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>41440</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>94.8</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>41470</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>95.4</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>41501</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>95.3</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>41532</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>95.7</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>41562</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>95.2</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>41593</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>96.3</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>41623</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>95.4</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>41654</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>95.8</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>41685</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>96.3</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>41713</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>96.9</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>41744</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>96.2</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>41774</v>
       </c>
@@ -1200,7 +1200,7 @@
         <v>95.6</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>41805</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>41835</v>
       </c>
@@ -1216,7 +1216,7 @@
         <v>95.5</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>41866</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>97.1</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>41897</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>95.8</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>41927</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>41958</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>96.7</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>41988</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>96.7</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>42019</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>98.6</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>42050</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>98.7</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>42078</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>98.3</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>42109</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>99.1</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>42139</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>100.4</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>42170</v>
       </c>
@@ -1304,7 +1304,7 @@
         <v>99.7</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>42200</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>42231</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>100.7</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>42262</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>100.8</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>42292</v>
       </c>
@@ -1336,7 +1336,7 @@
         <v>100.8</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>42323</v>
       </c>
@@ -1344,7 +1344,7 @@
         <v>100.6</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>42353</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>102.3</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>42384</v>
       </c>
@@ -1360,7 +1360,7 @@
         <v>101.9</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>42415</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>101.3</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>42444</v>
       </c>
@@ -1376,7 +1376,7 @@
         <v>100.9</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>42475</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>100.8</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>42505</v>
       </c>
@@ -1392,7 +1392,7 @@
         <v>101.4</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>42536</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>42566</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>102.3</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>42597</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>102.5</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>42628</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>101.3</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>42658</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>104.6</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>42689</v>
       </c>
@@ -1440,7 +1440,7 @@
         <v>102.3</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>42719</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>105.1</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>42750</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>103.1</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>42781</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>103.7</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <v>42809</v>
       </c>
@@ -1472,7 +1472,7 @@
         <v>106.4</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>42840</v>
       </c>
@@ -1480,7 +1480,7 @@
         <v>104.7</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <v>42870</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>105.7</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>42901</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>42931</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>105.9</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <v>42962</v>
       </c>
@@ -1512,7 +1512,7 @@
         <v>105.3</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>42993</v>
       </c>
@@ -1520,7 +1520,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>43023</v>
       </c>
@@ -1528,7 +1528,7 @@
         <v>105.7</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>43054</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>106.8</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
         <v>43084</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
         <v>43115</v>
       </c>
@@ -1552,7 +1552,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" s="1">
         <v>43146</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>105.1</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
         <v>43174</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>106.3</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <v>43205</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>109.3</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" s="1">
         <v>43235</v>
       </c>
@@ -1584,7 +1584,7 @@
         <v>107.1</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" s="1">
         <v>43266</v>
       </c>
@@ -1592,7 +1592,7 @@
         <v>108.1</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" s="1">
         <v>43296</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" s="1">
         <v>43327</v>
       </c>
@@ -1608,7 +1608,7 @@
         <v>107.3</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" s="1">
         <v>43358</v>
       </c>
@@ -1616,7 +1616,7 @@
         <v>107.4</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" s="1">
         <v>43388</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" s="1">
         <v>43419</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>108.7</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" s="1">
         <v>43449</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>108.3</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" s="1">
         <v>43480</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>109.9</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" s="1">
         <v>43511</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>110.3</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" s="1">
         <v>43539</v>
       </c>
@@ -1664,7 +1664,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161" s="1">
         <v>43570</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>110.6</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" s="1">
         <v>43600</v>
       </c>
@@ -1680,7 +1680,7 @@
         <v>108.9</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163" s="1">
         <v>43631</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>112.4</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164" s="1">
         <v>43661</v>
       </c>
@@ -1696,7 +1696,7 @@
         <v>111.7</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A165" s="1">
         <v>43692</v>
       </c>
@@ -1704,7 +1704,7 @@
         <v>111.1</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166" s="1">
         <v>43723</v>
       </c>
@@ -1712,7 +1712,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167" s="1">
         <v>43753</v>
       </c>
@@ -1720,7 +1720,7 @@
         <v>110.3</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168" s="1">
         <v>43784</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v>112.4</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169" s="1">
         <v>43814</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>111.2</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170" s="1">
         <v>43845</v>
       </c>
@@ -1744,7 +1744,7 @@
         <v>112.2</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171" s="1">
         <v>43876</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>112.6</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172" s="1">
         <v>43905</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>111.8</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A173" s="1">
         <v>43936</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>104.7</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174" s="1">
         <v>43966</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>117.8</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A175" s="1">
         <v>43997</v>
       </c>
@@ -1784,7 +1784,7 @@
         <v>117.1</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176" s="1">
         <v>44027</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>117.3</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177" s="1">
         <v>44058</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>118.8</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A178" s="1">
         <v>44089</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>117.9</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A179" s="1">
         <v>44119</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>120.1</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A180" s="1">
         <v>44150</v>
       </c>
@@ -1824,7 +1824,7 @@
         <v>123.1</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A181" s="1">
         <v>44180</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>113.3</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A182" s="1">
         <v>44211</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>106.3</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A183" s="1">
         <v>44242</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>110.1</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184" s="1">
         <v>44270</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>120.6</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185" s="1">
         <v>44301</v>
       </c>
@@ -1864,7 +1864,7 @@
         <v>112.7</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" s="1">
         <v>44331</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A187" s="1">
         <v>44362</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>123.5</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188" s="1">
         <v>44392</v>
       </c>
@@ -1888,7 +1888,7 @@
         <v>118.4</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189" s="1">
         <v>44423</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>119.8</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A190" s="1">
         <v>44454</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A191" s="1">
         <v>44484</v>
       </c>
@@ -1914,8 +1914,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <customProperties>
-    <customPr name="REFI_OFFICE_FUNCTION_DATA" r:id="rId1"/>
-  </customProperties>
 </worksheet>
 </file>
</xml_diff>